<commit_message>
fix remote data.json sherlock's file url
</commit_message>
<xml_diff>
--- a/data/collector/fs0c131y/fs0c131y.xlsx
+++ b/data/collector/fs0c131y/fs0c131y.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Status</t>
   </si>
@@ -48,9 +48,15 @@
     <t>Imgur</t>
   </si>
   <si>
+    <t>Keybase</t>
+  </si>
+  <si>
     <t>Pastebin</t>
   </si>
   <si>
+    <t>TradingView</t>
+  </si>
+  <si>
     <t>HackerOne</t>
   </si>
   <si>
@@ -60,70 +66,70 @@
     <t>HackerNews</t>
   </si>
   <si>
+    <t>TikTok</t>
+  </si>
+  <si>
+    <t>Dribbble</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Duolingo</t>
+  </si>
+  <si>
+    <t>Docker Hub</t>
+  </si>
+  <si>
     <t>Facebook</t>
   </si>
   <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>Codechef</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>Blogger</t>
+  </si>
+  <si>
+    <t>Disqus</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>Twitter</t>
+  </si>
+  <si>
     <t>IFTTT</t>
   </si>
   <si>
-    <t>Docker Hub</t>
-  </si>
-  <si>
-    <t>LeetCode</t>
-  </si>
-  <si>
-    <t>Codechef</t>
-  </si>
-  <si>
-    <t>PayPal</t>
-  </si>
-  <si>
-    <t>Keybase</t>
+    <t>SoundCloud</t>
+  </si>
+  <si>
+    <t>SteamGroup</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>AskFM</t>
+  </si>
+  <si>
+    <t>Twitch</t>
   </si>
   <si>
     <t>GitHub</t>
-  </si>
-  <si>
-    <t>TradingView</t>
-  </si>
-  <si>
-    <t>SteamGroup</t>
-  </si>
-  <si>
-    <t>Disqus</t>
-  </si>
-  <si>
-    <t>TikTok</t>
-  </si>
-  <si>
-    <t>Twitter</t>
-  </si>
-  <si>
-    <t>VK</t>
-  </si>
-  <si>
-    <t>Dribbble</t>
-  </si>
-  <si>
-    <t>AskFM</t>
-  </si>
-  <si>
-    <t>Instagram</t>
-  </si>
-  <si>
-    <t>Blogger</t>
-  </si>
-  <si>
-    <t>Twitch</t>
-  </si>
-  <si>
-    <t>Steam</t>
-  </si>
-  <si>
-    <t>Reddit</t>
-  </si>
-  <si>
-    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -952,6 +958,36 @@
         <v>8</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="1" t="s"/>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="1" t="s"/>
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>